<commit_message>
Add spider to get graphic links
</commit_message>
<xml_diff>
--- a/TermFrequencyMatrix.xlsx
+++ b/TermFrequencyMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrohenkel/Documents/SMU/IR/project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1EA71EBA-CD00-0643-877B-E9659AC05387}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EA54F34D-1C79-4A48-8AF2-9EC32A928894}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="17060"/>
   </bookViews>
@@ -8710,7 +8710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AD1" sqref="AD1:AE2"/>
     </sheetView>
   </sheetViews>

</xml_diff>